<commit_message>
Suggestion goal spec is working
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakerowley/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clabesse/Sites/lewagon/clique-connect/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DBFD43-BDA8-1241-83B4-88D43CA61DA5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Businesses" sheetId="1" r:id="rId1"/>
     <sheet name="Clicks" sheetId="2" r:id="rId2"/>
     <sheet name="Suggestions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="134">
   <si>
     <t>name</t>
   </si>
@@ -75,9 +74,6 @@
   </si>
   <si>
     <t>Tinder</t>
-  </si>
-  <si>
-    <t>Atlassian</t>
   </si>
   <si>
     <t>Dating
@@ -701,11 +697,14 @@
     <t>Deliveroo
 Uber Eats</t>
   </si>
+  <si>
+    <t>Event Cinema</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -742,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -755,6 +754,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,10 +1035,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1084,684 +1085,684 @@
         <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
-        <v>72</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
         <v>121</v>
       </c>
-      <c r="C29" t="s">
-        <v>122</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1771,7 +1772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="333" zoomScalePageLayoutView="333" workbookViewId="0">
@@ -1822,54 +1823,133 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D54D736-1D58-884E-BD55-A61361365596}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A2:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="6">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="6">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="6">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="6">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="6">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="6">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="6">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="6">
         <v>9</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
search page now has images
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakerowley/code/clique-connect/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33030184-98FA-2C46-A11B-7AE303751B68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C1FEFE-7A4B-3E49-BBF5-639AFAFA8AA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2258,9 +2258,6 @@
     <t>https://www.cliquelabs.com/wp-content/uploads/2018/03/logo-1-e1523772838215.png</t>
   </si>
   <si>
-    <t>https://www.tribegroup.co/hs-fs/hubfs/Tribe%202017/Images/logo.png?t=1523949699735&amp;width=666&amp;name=logo.png</t>
-  </si>
-  <si>
     <t>http://vamp.wpengine.com/wp-content/uploads/2015/12/logo.vamp_.svg</t>
   </si>
   <si>
@@ -2276,9 +2273,6 @@
     <t>http://media.globaldatinginsights.com/wp-content/uploads/2016/01/18223915/bee.png</t>
   </si>
   <si>
-    <t>https://designerex.com.au/assets/logo2-1ffc7ca7a093c4d36451efbffe32a8f6f72f8cea45bde6e78bc550aa3c768370.png</t>
-  </si>
-  <si>
     <t>https://s3.producthunt.com/static/ph-logo-1.png</t>
   </si>
   <si>
@@ -2439,6 +2433,12 @@
   </si>
   <si>
     <t>https://d2hzvxamqgodh.cloudfront.net/sites/default/files/storelogo/nbn.jpg</t>
+  </si>
+  <si>
+    <t>http://tylerbdesigns.com/images/portfolio/tribe/tribe-logo.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/6rZ9tMI9rlY/maxresdefault.jpg</t>
   </si>
 </sst>
 </file>
@@ -2909,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J60" zoomScale="113" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="K16" zoomScale="113" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2964,7 +2964,7 @@
         <v>359</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
@@ -3002,7 +3002,7 @@
         <v>358</v>
       </c>
       <c r="L2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="368" x14ac:dyDescent="0.2">
@@ -3040,7 +3040,7 @@
         <v>360</v>
       </c>
       <c r="L3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -3078,7 +3078,7 @@
         <v>361</v>
       </c>
       <c r="L4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="176" x14ac:dyDescent="0.2">
@@ -3116,7 +3116,7 @@
         <v>362</v>
       </c>
       <c r="L5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="144" x14ac:dyDescent="0.2">
@@ -3154,7 +3154,7 @@
         <v>363</v>
       </c>
       <c r="L6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="320" x14ac:dyDescent="0.2">
@@ -3192,7 +3192,7 @@
         <v>364</v>
       </c>
       <c r="L7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="192" x14ac:dyDescent="0.2">
@@ -3230,7 +3230,7 @@
         <v>365</v>
       </c>
       <c r="L8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="192" x14ac:dyDescent="0.2">
@@ -3268,7 +3268,7 @@
         <v>366</v>
       </c>
       <c r="L9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="288" x14ac:dyDescent="0.2">
@@ -3306,7 +3306,7 @@
         <v>367</v>
       </c>
       <c r="L10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="176" x14ac:dyDescent="0.2">
@@ -3341,10 +3341,10 @@
         <v>76</v>
       </c>
       <c r="K11" t="s">
-        <v>368</v>
+        <v>427</v>
       </c>
       <c r="L11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="176" x14ac:dyDescent="0.2">
@@ -3379,10 +3379,10 @@
         <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="384" x14ac:dyDescent="0.2">
@@ -3417,10 +3417,10 @@
         <v>87</v>
       </c>
       <c r="K13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -3455,10 +3455,10 @@
         <v>94</v>
       </c>
       <c r="K14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="256" x14ac:dyDescent="0.2">
@@ -3493,10 +3493,10 @@
         <v>99</v>
       </c>
       <c r="K15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="288" x14ac:dyDescent="0.2">
@@ -3529,10 +3529,10 @@
         <v>102</v>
       </c>
       <c r="K16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L16" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="160" x14ac:dyDescent="0.2">
@@ -3567,10 +3567,10 @@
         <v>107</v>
       </c>
       <c r="K17" t="s">
-        <v>374</v>
+        <v>428</v>
       </c>
       <c r="L17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="288" x14ac:dyDescent="0.2">
@@ -3605,10 +3605,10 @@
         <v>111</v>
       </c>
       <c r="K18" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L18" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="224" x14ac:dyDescent="0.2">
@@ -3643,10 +3643,10 @@
         <v>117</v>
       </c>
       <c r="K19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="144" x14ac:dyDescent="0.2">
@@ -3681,10 +3681,10 @@
         <v>123</v>
       </c>
       <c r="K20" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -3719,10 +3719,10 @@
         <v>127</v>
       </c>
       <c r="K21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L21" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="160" x14ac:dyDescent="0.2">
@@ -3757,10 +3757,10 @@
         <v>134</v>
       </c>
       <c r="K22" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L22" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="160" x14ac:dyDescent="0.2">
@@ -3793,10 +3793,10 @@
         <v>139</v>
       </c>
       <c r="K23" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="256" x14ac:dyDescent="0.2">
@@ -3831,10 +3831,10 @@
         <v>145</v>
       </c>
       <c r="K24" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L24" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="208" x14ac:dyDescent="0.2">
@@ -3869,10 +3869,10 @@
         <v>151</v>
       </c>
       <c r="K25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -3907,10 +3907,10 @@
         <v>156</v>
       </c>
       <c r="K26" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L26" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="320" x14ac:dyDescent="0.2">
@@ -3943,10 +3943,10 @@
         <v>161</v>
       </c>
       <c r="K27" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L27" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -3979,10 +3979,10 @@
         <v>166</v>
       </c>
       <c r="K28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L28" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4015,10 +4015,10 @@
         <v>172</v>
       </c>
       <c r="K29" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L29" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4051,10 +4051,10 @@
         <v>178</v>
       </c>
       <c r="K30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L30" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="208" x14ac:dyDescent="0.2">
@@ -4087,10 +4087,10 @@
         <v>184</v>
       </c>
       <c r="K31" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L31" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="144" x14ac:dyDescent="0.2">
@@ -4123,10 +4123,10 @@
         <v>189</v>
       </c>
       <c r="K32" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L32" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4159,10 +4159,10 @@
         <v>193</v>
       </c>
       <c r="K33" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L33" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4195,10 +4195,10 @@
         <v>199</v>
       </c>
       <c r="K34" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L34" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="224" x14ac:dyDescent="0.2">
@@ -4231,10 +4231,10 @@
         <v>205</v>
       </c>
       <c r="K35" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L35" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4267,10 +4267,10 @@
         <v>209</v>
       </c>
       <c r="K36" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L36" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="176" x14ac:dyDescent="0.2">
@@ -4303,10 +4303,10 @@
         <v>212</v>
       </c>
       <c r="K37" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L37" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="208" x14ac:dyDescent="0.2">
@@ -4337,10 +4337,10 @@
         <v>217</v>
       </c>
       <c r="K38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L38" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4373,10 +4373,10 @@
         <v>338</v>
       </c>
       <c r="K39" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L39" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4407,10 +4407,10 @@
         <v>339</v>
       </c>
       <c r="K40" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L40" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4443,10 +4443,10 @@
         <v>340</v>
       </c>
       <c r="K41" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L41" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4479,10 +4479,10 @@
         <v>341</v>
       </c>
       <c r="K42" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L42" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="256" x14ac:dyDescent="0.2">
@@ -4515,10 +4515,10 @@
         <v>342</v>
       </c>
       <c r="K43" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L43" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4548,10 +4548,10 @@
         <v>239</v>
       </c>
       <c r="K44" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L44" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="176" x14ac:dyDescent="0.2">
@@ -4581,10 +4581,10 @@
         <v>241</v>
       </c>
       <c r="K45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L45" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4619,10 +4619,10 @@
         <v>335</v>
       </c>
       <c r="K46" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L46" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4655,10 +4655,10 @@
         <v>343</v>
       </c>
       <c r="K47" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L47" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4691,10 +4691,10 @@
         <v>344</v>
       </c>
       <c r="K48" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L48" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4724,10 +4724,10 @@
         <v>255</v>
       </c>
       <c r="K49" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L49" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="256" x14ac:dyDescent="0.2">
@@ -4757,10 +4757,10 @@
         <v>258</v>
       </c>
       <c r="K50" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="L50" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="160" x14ac:dyDescent="0.2">
@@ -4792,10 +4792,10 @@
         <v>264</v>
       </c>
       <c r="K51" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L51" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
@@ -4830,10 +4830,10 @@
         <v>345</v>
       </c>
       <c r="K52" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="L52" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -4866,10 +4866,10 @@
         <v>346</v>
       </c>
       <c r="K53" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L53" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="176" x14ac:dyDescent="0.2">
@@ -4904,10 +4904,10 @@
         <v>347</v>
       </c>
       <c r="K54" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L54" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="224" x14ac:dyDescent="0.2">
@@ -4942,10 +4942,10 @@
         <v>348</v>
       </c>
       <c r="K55" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L55" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="224" x14ac:dyDescent="0.2">
@@ -4980,10 +4980,10 @@
         <v>349</v>
       </c>
       <c r="K56" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L56" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="224" x14ac:dyDescent="0.2">
@@ -5018,10 +5018,10 @@
         <v>350</v>
       </c>
       <c r="K57" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="L57" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="160" x14ac:dyDescent="0.2">
@@ -5056,10 +5056,10 @@
         <v>351</v>
       </c>
       <c r="K58" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="L58" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -5092,10 +5092,10 @@
         <v>352</v>
       </c>
       <c r="K59" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L59" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="160" x14ac:dyDescent="0.2">
@@ -5127,10 +5127,10 @@
         <v>302</v>
       </c>
       <c r="K60" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L60" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -5165,10 +5165,10 @@
         <v>353</v>
       </c>
       <c r="K61" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L61" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -5201,10 +5201,10 @@
         <v>354</v>
       </c>
       <c r="K62" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="L62" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -5239,10 +5239,10 @@
         <v>355</v>
       </c>
       <c r="K63" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="L63" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -5277,10 +5277,10 @@
         <v>356</v>
       </c>
       <c r="K64" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L64" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="240" x14ac:dyDescent="0.2">
@@ -5313,10 +5313,10 @@
         <v>357</v>
       </c>
       <c r="K65" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="L65" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="128" x14ac:dyDescent="0.2">
@@ -5348,10 +5348,10 @@
         <v>329</v>
       </c>
       <c r="K66" t="s">
+        <v>418</v>
+      </c>
+      <c r="L66" t="s">
         <v>420</v>
-      </c>
-      <c r="L66" t="s">
-        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ford to match list
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="435">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -99,7 +99,7 @@
 Event Cinema
 Gather Online
 Clique Labs
-</t>
+Ford</t>
   </si>
   <si>
     <t xml:space="preserve">Hoyts Group
@@ -107,33 +107,45 @@
 Deliveroo</t>
   </si>
   <si>
-    <t xml:space="preserve">Sport
-Health
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Image
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fun
+Explore
+Brands
+Sport
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Health
 Running
 Fashion
-Cosmetics
-Beauty
 Nightlife
-Zoho
-London
-Dogs
-Netflix
-Amazon
-Hipster
-Beach
-Dating
-Clubbing
-Dogs
-Marathons
-Friends
-Summer
 Holidays
-Sport
-Fashion
-Vouge
-Prada
-Westfield
 </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://tinder.com/</t>
@@ -2421,6 +2433,88 @@
     <t xml:space="preserve">https://s3.amazonaws.com/au-tm/1814983.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">Ford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicles
+Manufacturing
+Transport
+Sales</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clique Labs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Mad Paws
+Hoyts Group
+Event Cinema
+Gather Online</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Image
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fun
+Explore
+Brands
+Sport
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Health
+Running
+Fashion
+Nightlife
+Holidays
+Cars
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ford.com.au/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/d/d8/Ford_logo.svg/2000px-Ford_logo.svg.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">clicker</t>
   </si>
   <si>
@@ -2445,7 +2539,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MMM\-YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2467,6 +2561,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -2518,11 +2618,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2555,20 +2655,28 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2661,10 +2769,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H51" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K52" activeCellId="0" sqref="K52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2720,7 +2828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="172.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2733,7 +2841,7 @@
       <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -5104,6 +5212,44 @@
         <v>423</v>
       </c>
       <c r="L66" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="186.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="L67" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5130,7 +5276,7 @@
   <dimension ref="A1:M164"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="8:8 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -5142,13 +5288,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5381,20 +5527,20 @@
       <c r="C22" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="14" t="s">
         <v>101</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -5416,7 +5562,7 @@
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -5427,7 +5573,7 @@
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -5438,7 +5584,7 @@
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="14" t="s">
         <v>238</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -5460,7 +5606,7 @@
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="14" t="s">
         <v>250</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -5471,7 +5617,7 @@
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="14" t="s">
         <v>199</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -5482,7 +5628,7 @@
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="14" t="s">
         <v>174</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -5493,7 +5639,7 @@
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -5766,27 +5912,27 @@
       <c r="A56" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E56" s="13"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="12"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="15" t="s">
         <v>412</v>
       </c>
       <c r="C57" s="0" t="n">
@@ -5797,7 +5943,7 @@
       <c r="A58" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="14" t="s">
         <v>324</v>
       </c>
       <c r="C58" s="0" t="n">
@@ -5808,7 +5954,7 @@
       <c r="A59" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="0" t="n">
@@ -5819,7 +5965,7 @@
       <c r="A60" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="14" t="s">
         <v>357</v>
       </c>
       <c r="C60" s="0" t="n">
@@ -5830,7 +5976,7 @@
       <c r="A61" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="14" t="s">
         <v>51</v>
       </c>
       <c r="C61" s="0" t="n">
@@ -5852,7 +5998,7 @@
       <c r="A63" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="15" t="s">
         <v>359</v>
       </c>
       <c r="C63" s="0" t="n">
@@ -5863,7 +6009,7 @@
       <c r="A64" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="14" t="s">
         <v>206</v>
       </c>
       <c r="C64" s="0" t="n">
@@ -6639,7 +6785,7 @@
       <c r="A133" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="B133" s="15" t="s">
         <v>357</v>
       </c>
       <c r="C133" s="0" t="n">
@@ -6650,7 +6796,7 @@
       <c r="A134" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B134" s="15" t="s">
         <v>375</v>
       </c>
       <c r="C134" s="0" t="n">
@@ -6672,7 +6818,7 @@
       <c r="A136" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="15" t="s">
         <v>399</v>
       </c>
       <c r="C136" s="0" t="n">
@@ -6705,7 +6851,7 @@
       <c r="A139" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B139" s="12" t="s">
+      <c r="B139" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C139" s="0" t="n">
@@ -6716,7 +6862,7 @@
       <c r="A140" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B140" s="14" t="s">
         <v>101</v>
       </c>
       <c r="C140" s="0" t="n">
@@ -6727,7 +6873,7 @@
       <c r="A141" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B141" s="12" t="s">
+      <c r="B141" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C141" s="0" t="n">
@@ -6738,7 +6884,7 @@
       <c r="A142" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B142" s="12" t="s">
+      <c r="B142" s="14" t="s">
         <v>295</v>
       </c>
       <c r="C142" s="0" t="n">
@@ -6881,7 +7027,7 @@
       <c r="A155" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B155" s="13" t="s">
+      <c r="B155" s="15" t="s">
         <v>278</v>
       </c>
       <c r="C155" s="0" t="n">
@@ -6892,7 +7038,7 @@
       <c r="A156" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B156" s="13" t="s">
+      <c r="B156" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C156" s="0" t="n">
@@ -6903,7 +7049,7 @@
       <c r="A157" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B157" s="12" t="s">
+      <c r="B157" s="14" t="s">
         <v>101</v>
       </c>
       <c r="C157" s="0" t="n">
@@ -6914,7 +7060,7 @@
       <c r="A158" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B158" s="12" t="s">
+      <c r="B158" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C158" s="0" t="n">
@@ -6925,7 +7071,7 @@
       <c r="A159" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B159" s="12" t="s">
+      <c r="B159" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C159" s="0" t="n">
@@ -6936,7 +7082,7 @@
       <c r="A160" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B160" s="12" t="s">
+      <c r="B160" s="14" t="s">
         <v>134</v>
       </c>
       <c r="C160" s="0" t="n">
@@ -6958,7 +7104,7 @@
       <c r="A162" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B162" s="13" t="s">
+      <c r="B162" s="15" t="s">
         <v>312</v>
       </c>
       <c r="C162" s="0" t="n">
@@ -6969,7 +7115,7 @@
       <c r="A163" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B163" s="13" t="s">
+      <c r="B163" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C163" s="0" t="n">
@@ -6980,7 +7126,7 @@
       <c r="A164" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B164" s="12" t="s">
+      <c r="B164" s="14" t="s">
         <v>213</v>
       </c>
       <c r="C164" s="0" t="n">
@@ -7006,58 +7152,58 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="8:8 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="15.9740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="11.8555555555556"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="16" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="3.33333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="16" width="12.2481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="B1" s="12" t="n">
+      <c r="A1" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="n">
+      <c r="C1" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="n">
+      <c r="D1" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="n">
+      <c r="E1" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="n">
+      <c r="F1" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="n">
+      <c r="G1" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="n">
+      <c r="H1" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="n">
+      <c r="I1" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="n">
+      <c r="J1" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="n">
+      <c r="K1" s="14" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7065,188 +7211,188 @@
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="14" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="14" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>295</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="14" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="14" t="s">
         <v>238</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>134</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="14" t="s">
         <v>105</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -7258,16 +7404,16 @@
       <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="14" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7278,10 +7424,10 @@
       <c r="B8" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="14" t="s">
         <v>231</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -7293,16 +7439,16 @@
       <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="15" t="s">
         <v>299</v>
       </c>
     </row>
@@ -7310,34 +7456,34 @@
       <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="14" t="s">
         <v>174</v>
       </c>
     </row>
@@ -7345,34 +7491,34 @@
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>428</v>
+      <c r="G10" s="14" t="s">
+        <v>434</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="14" t="s">
         <v>213</v>
       </c>
     </row>
@@ -7380,16 +7526,16 @@
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="15" t="s">
         <v>375</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="15" t="s">
         <v>399</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -7398,16 +7544,16 @@
       <c r="G11" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="14" t="s">
         <v>295</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test demo cases
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -115,7 +115,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Image
+      <t xml:space="preserve">Health
+Running
+Fashion
+Nightlife
+Holidays
 </t>
     </r>
     <r>
@@ -125,26 +129,11 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Fun
+      <t xml:space="preserve">Image
+Fun
 Explore
 Brands
-Sport
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Health
-Running
-Fashion
-Nightlife
-Holidays
-</t>
+Sport</t>
     </r>
   </si>
   <si>
@@ -436,7 +425,7 @@
     <t xml:space="preserve">https://www.gatheronline.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.gatheronline.com/web/images/icons/logo.svg</t>
+    <t xml:space="preserve">https://www.thehappierhomemaker.com/wp-content/uploads/2017/09/gather-printable.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Fashion
@@ -493,7 +482,7 @@
     <t xml:space="preserve">https://www.glamcorner.com.au/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.glamcorner.com.au/skin/frontend/glamcorner/default/images/logo.svg</t>
+    <t xml:space="preserve">http://www.dealsland.com.au/wp-content/uploads/2015/06/glamcorner_coupon_code.png</t>
   </si>
   <si>
     <t xml:space="preserve">England</t>
@@ -582,7 +571,7 @@
     <t xml:space="preserve">https://www.tribegroup.co/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.tribegroup.co/hs-fs/hubfs/Tribe%202017/Images/logo.png?t=1523949699735&amp;width=666&amp;name=logo.png</t>
+    <t xml:space="preserve">https://d3p157427w54jq.cloudfront.net/uploads/2018/04/TRIBELogotype-RGB-V-FC-2-400x288.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Visual Amplifiers</t>
@@ -2137,7 +2126,7 @@
     <t xml:space="preserve">https://hismileteeth.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://cdn.shopify.com/s/files/1/2502/5300/files/text.svg</t>
+    <t xml:space="preserve">https://i.ytimg.com/vi/XTO4JyeWxKU/maxresdefault.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Little Cuggles
@@ -2475,7 +2464,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Image
+      <t xml:space="preserve">Health
+Running
+Nightlife
+Holidays
+Cars
 </t>
     </r>
     <r>
@@ -2485,26 +2478,11 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Fun
+      <t xml:space="preserve">Image
+Fun
 Explore
 Brands
 Sport
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Health
-Running
-Fashion
-Nightlife
-Holidays
-Cars
 </t>
     </r>
   </si>
@@ -2771,8 +2749,8 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I56" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2828,7 +2806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="172.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="144.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3056,7 +3034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="192" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="171.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -3094,7 +3072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="192" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="172.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -3170,7 +3148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="176" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="157.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>86</v>
       </c>
@@ -5215,7 +5193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="186.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="158.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>424</v>
       </c>
@@ -5255,8 +5233,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J15" r:id="rId1" display="https://www.happn.com/en/"/>
-    <hyperlink ref="J46" r:id="rId2" display="http://www.nudie.com.au/"/>
+    <hyperlink ref="K9" r:id="rId1" display="http://www.dealsland.com.au/wp-content/uploads/2015/06/glamcorner_coupon_code.png"/>
+    <hyperlink ref="J15" r:id="rId2" display="https://www.happn.com/en/"/>
+    <hyperlink ref="J46" r:id="rId3" display="http://www.nudie.com.au/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5276,7 +5255,7 @@
   <dimension ref="A1:M164"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="8:8 B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -7152,7 +7131,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="8:8 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>

</xml_diff>

<commit_message>
added notes functionality onto the show page for each business
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -107,34 +107,16 @@
 Deliveroo</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Health
+    <t xml:space="preserve">Health
 Running
 Fashion
 Nightlife
 Holidays
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Image
+Image
 Fun
 Explore
 Brands
 Sport</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">https://tinder.com/</t>
@@ -2431,60 +2413,24 @@
 Sales</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Clique Labs
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Mad Paws
+    <t xml:space="preserve">Clique Labs
+Mad Paws
 Hoyts Group
 Event Cinema
 Gather Online</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Health
+  </si>
+  <si>
+    <t xml:space="preserve">Health
 Running
 Nightlife
 Holidays
 Cars
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Image
+Image
 Fun
 Explore
 Brands
 Sport
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">https://www.ford.com.au/</t>
@@ -2517,7 +2463,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MMM\-YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2539,12 +2485,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -2596,11 +2536,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2633,28 +2573,20 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2749,23 +2681,24 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I56" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.162962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4148,7 +4081,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="208" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="186.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>254</v>
       </c>
@@ -5197,7 +5130,7 @@
       <c r="A67" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="5" t="s">
         <v>425</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -5209,13 +5142,13 @@
       <c r="E67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="5" t="s">
         <v>426</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="13" t="s">
+      <c r="H67" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I67" s="1" t="s">
@@ -5260,9 +5193,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.56666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.76296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5506,20 +5440,20 @@
       <c r="C22" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -5541,7 +5475,7 @@
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>119</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -5552,7 +5486,7 @@
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -5563,7 +5497,7 @@
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>238</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -5585,7 +5519,7 @@
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="12" t="s">
         <v>250</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -5596,7 +5530,7 @@
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>199</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -5607,7 +5541,7 @@
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="12" t="s">
         <v>174</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -5618,7 +5552,7 @@
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -5891,27 +5825,27 @@
       <c r="A56" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E56" s="15"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="15"/>
-      <c r="M56" s="14"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="12"/>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="13" t="s">
         <v>412</v>
       </c>
       <c r="C57" s="0" t="n">
@@ -5922,7 +5856,7 @@
       <c r="A58" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C58" s="0" t="n">
@@ -5933,7 +5867,7 @@
       <c r="A59" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="0" t="n">
@@ -5944,7 +5878,7 @@
       <c r="A60" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="12" t="s">
         <v>357</v>
       </c>
       <c r="C60" s="0" t="n">
@@ -5955,7 +5889,7 @@
       <c r="A61" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C61" s="0" t="n">
@@ -5977,7 +5911,7 @@
       <c r="A63" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="13" t="s">
         <v>359</v>
       </c>
       <c r="C63" s="0" t="n">
@@ -5988,7 +5922,7 @@
       <c r="A64" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="12" t="s">
         <v>206</v>
       </c>
       <c r="C64" s="0" t="n">
@@ -6764,7 +6698,7 @@
       <c r="A133" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B133" s="15" t="s">
+      <c r="B133" s="13" t="s">
         <v>357</v>
       </c>
       <c r="C133" s="0" t="n">
@@ -6775,7 +6709,7 @@
       <c r="A134" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="13" t="s">
         <v>375</v>
       </c>
       <c r="C134" s="0" t="n">
@@ -6797,7 +6731,7 @@
       <c r="A136" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B136" s="15" t="s">
+      <c r="B136" s="13" t="s">
         <v>399</v>
       </c>
       <c r="C136" s="0" t="n">
@@ -6830,7 +6764,7 @@
       <c r="A139" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B139" s="14" t="s">
+      <c r="B139" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C139" s="0" t="n">
@@ -6841,7 +6775,7 @@
       <c r="A140" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B140" s="14" t="s">
+      <c r="B140" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C140" s="0" t="n">
@@ -6852,7 +6786,7 @@
       <c r="A141" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B141" s="14" t="s">
+      <c r="B141" s="12" t="s">
         <v>119</v>
       </c>
       <c r="C141" s="0" t="n">
@@ -6863,7 +6797,7 @@
       <c r="A142" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B142" s="12" t="s">
         <v>295</v>
       </c>
       <c r="C142" s="0" t="n">
@@ -7006,7 +6940,7 @@
       <c r="A155" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B155" s="15" t="s">
+      <c r="B155" s="13" t="s">
         <v>278</v>
       </c>
       <c r="C155" s="0" t="n">
@@ -7017,7 +6951,7 @@
       <c r="A156" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B156" s="15" t="s">
+      <c r="B156" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C156" s="0" t="n">
@@ -7028,7 +6962,7 @@
       <c r="A157" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B157" s="14" t="s">
+      <c r="B157" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C157" s="0" t="n">
@@ -7039,7 +6973,7 @@
       <c r="A158" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C158" s="0" t="n">
@@ -7050,7 +6984,7 @@
       <c r="A159" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B159" s="14" t="s">
+      <c r="B159" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C159" s="0" t="n">
@@ -7061,7 +6995,7 @@
       <c r="A160" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B160" s="14" t="s">
+      <c r="B160" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C160" s="0" t="n">
@@ -7083,7 +7017,7 @@
       <c r="A162" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B162" s="15" t="s">
+      <c r="B162" s="13" t="s">
         <v>312</v>
       </c>
       <c r="C162" s="0" t="n">
@@ -7094,7 +7028,7 @@
       <c r="A163" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B163" s="15" t="s">
+      <c r="B163" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C163" s="0" t="n">
@@ -7105,7 +7039,7 @@
       <c r="A164" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B164" s="14" t="s">
+      <c r="B164" s="12" t="s">
         <v>213</v>
       </c>
       <c r="C164" s="0" t="n">
@@ -7136,53 +7070,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="16" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="16" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="14.6"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="3.33333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.4444444444444"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="B1" s="14" t="n">
+      <c r="B1" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="n">
+      <c r="C1" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="n">
+      <c r="D1" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="n">
+      <c r="E1" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="n">
+      <c r="F1" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="n">
+      <c r="G1" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="n">
+      <c r="H1" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="n">
+      <c r="I1" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="n">
+      <c r="J1" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="n">
+      <c r="K1" s="12" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7190,188 +7124,188 @@
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="12" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="12" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>295</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>238</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>134</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -7383,16 +7317,16 @@
       <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="12" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7403,10 +7337,10 @@
       <c r="B8" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>231</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -7418,16 +7352,16 @@
       <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="13" t="s">
         <v>299</v>
       </c>
     </row>
@@ -7435,34 +7369,34 @@
       <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="12" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="12" t="s">
         <v>174</v>
       </c>
     </row>
@@ -7470,34 +7404,34 @@
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>434</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="12" t="s">
         <v>213</v>
       </c>
     </row>
@@ -7505,16 +7439,16 @@
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>375</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>399</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -7523,16 +7457,16 @@
       <c r="G11" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="12" t="s">
         <v>295</v>
       </c>
     </row>

</xml_diff>

<commit_message>
suggestions now tailored to user location and show the last ten daily suggestions for each user
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -1603,7 +1603,7 @@
     <t xml:space="preserve">http://keynected.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">http://kwkeyclub.weebly.com/uploads/8/5/4/8/85481056/remindapp_orig.png</t>
+    <t xml:space="preserve">https://kwkeyclub.weebly.com/uploads/8/5/4/8/85481056/remindapp_orig.png</t>
   </si>
   <si>
     <t xml:space="preserve">Paws for Life</t>
@@ -2052,7 +2052,7 @@
     <t xml:space="preserve">http://www.ozifyaustralia.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.ozifyaustralia.com/thumbnaillarge/logo.jpg</t>
+    <t xml:space="preserve">http://www.soultosole.com.au/thumbnaillarge/logo.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">HiSmile</t>
@@ -2681,24 +2681,24 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G55" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.162962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4185,7 +4185,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="128" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>263</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="224" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="199.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>350</v>
       </c>
@@ -5193,10 +5193,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.76296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.95925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7070,19 +7070,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.7"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="14.8962962962963"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="14" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.6407407407407"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update daily suggestions in now executed daily using a rake command from heroku scheduler
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -2681,8 +2681,8 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G55" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>

</xml_diff>

<commit_message>
continuing work on the confirmable users
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -2469,7 +2469,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2492,7 +2491,6 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2681,24 +2679,24 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4293,7 +4291,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="128" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>274</v>
       </c>
@@ -5193,10 +5191,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.15185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7070,19 +7068,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.7"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.7"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="15.2888888888889"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="14" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.837037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixed seed data and seed file
</commit_message>
<xml_diff>
--- a/db/Database.xlsx
+++ b/db/Database.xlsx
@@ -710,7 +710,7 @@
     <t xml:space="preserve">https://www.happn.com/en/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.happn.com/images/logo-happn-mini-laptop.svg</t>
+    <t xml:space="preserve">https://www.happn.com/static/images/logo-happn-mini-laptop.svg</t>
   </si>
   <si>
     <t xml:space="preserve">Bumble</t>
@@ -2052,7 +2052,7 @@
     <t xml:space="preserve">http://www.ozifyaustralia.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.soultosole.com.au/thumbnaillarge/logo.jpg</t>
+    <t xml:space="preserve">https://www.soultosole.com.au/thumbnaillarge/logo.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">HiSmile</t>
@@ -2681,24 +2681,24 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F55" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3233,7 +3233,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="256" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="229.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>101</v>
       </c>
@@ -5168,7 +5168,8 @@
   <hyperlinks>
     <hyperlink ref="K9" r:id="rId1" display="http://www.dealsland.com.au/wp-content/uploads/2015/06/glamcorner_coupon_code.png"/>
     <hyperlink ref="J15" r:id="rId2" display="https://www.happn.com/en/"/>
-    <hyperlink ref="J46" r:id="rId3" display="http://www.nudie.com.au/"/>
+    <hyperlink ref="K15" r:id="rId3" display="https://www.happn.com/static/images/logo-happn-mini-laptop.svg"/>
+    <hyperlink ref="J46" r:id="rId4" display="http://www.nudie.com.au/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5193,10 +5194,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.15185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7070,19 +7071,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.7"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.7"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="15.2888888888889"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="14" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="14" width="12.837037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>